<commit_message>
delete file,another one will add
</commit_message>
<xml_diff>
--- a/datas/test.xlsx
+++ b/datas/test.xlsx
@@ -1,74 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="0" windowWidth="19500" windowHeight="12620" tabRatio="500"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="联系人" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="联系人" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>aa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>cc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>zz</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>中国</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我爱祖国</t>
+  </si>
+  <si>
+    <t>2018-07-18 15:52:44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,16 +77,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="普通" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -418,20 +410,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1">
+      <c r="A1" t="n">
         <v>11</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="n">
         <v>55</v>
       </c>
       <c r="C1" t="s">
@@ -442,65 +438,67 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" t="n">
         <v>22</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" t="n">
         <v>33</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" t="n">
         <v>44</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>22</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" t="n">
         <v>55</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>